<commit_message>
JM added ProII files
</commit_message>
<xml_diff>
--- a/OIDs Template.xlsx
+++ b/OIDs Template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gutierrj\Downloads\data_transfer\data_transfer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gutierrj\source\data_transfer\data_transfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D47101-1666-480A-B796-A92A659875CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686EA505-94DF-4EEE-B857-209A388F0DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{92C1C962-718B-4E44-9E2C-823D9C78B2DC}"/>
+    <workbookView xWindow="17910" yWindow="2535" windowWidth="9735" windowHeight="11385" activeTab="2" xr2:uid="{92C1C962-718B-4E44-9E2C-823D9C78B2DC}"/>
   </bookViews>
   <sheets>
     <sheet name="HYSYS" sheetId="1" r:id="rId1"/>
     <sheet name="A+" sheetId="2" r:id="rId2"/>
+    <sheet name="ProII" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="61">
   <si>
     <t>Class</t>
   </si>
@@ -214,6 +215,12 @@
   </si>
   <si>
     <t>Distillation</t>
+  </si>
+  <si>
+    <t>Simple HX</t>
+  </si>
+  <si>
+    <t>Flash</t>
   </si>
 </sst>
 </file>
@@ -991,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67D9E2D-5B0D-474A-BD74-7FA7621D7432}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,4 +1538,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE46092-EE65-4F8F-907C-C8F2C5E00A70}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>